<commit_message>
mcu serial control option for LEDs
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-1/reference/Interface Bill of Materials v2.xlsx
+++ b/designs/Pufferfish-Interface-1/reference/Interface Bill of Materials v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-1/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785D15F5-41F4-3D4F-AD17-C55FA53870D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E37E20-B08C-F545-B615-0C9ADECFA6D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="460" windowWidth="25040" windowHeight="14040" xr2:uid="{AB4FADCF-5D3E-0F4F-A6DE-656B770204FC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
   <si>
     <t>ID</t>
   </si>
@@ -381,13 +381,33 @@
   </si>
   <si>
     <t>Solder lug terminals (3) --&gt; solder to wire --&gt; connect to PHR-3 then to CONN3</t>
+  </si>
+  <si>
+    <t>31-925</t>
+  </si>
+  <si>
+    <t>https://www.newark.com/eao/31-925/switch-guard/dp/50F8274?gclid=Cj0KCQjw3ZX4BRDmARIsAFYh7ZL4TmIx5-yMIRRJnkCFsqdzfS6YZAsvRjPKTaOv0U1XTDgEo3GKLyYaAg49EALw_wcB&amp;mckv=s6B25skjl_dc|pcrid|434136793434|plid||kword||match||slid||product|50F8274|pgrid|100464451146|ptaid|aud-905551039420:pla-904243529025|&amp;CMP=KNC-GUSA-GEN-Shopping-NewStructure-Switches-Relays</t>
+  </si>
+  <si>
+    <r>
+      <t>Switch Finger Guard,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF757575"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> EAO 31 Series Pushbutton Switches</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -497,6 +517,25 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF757575"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -528,12 +567,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -560,6 +600,8 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -875,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB09F318-339D-2C4D-BE3F-E973DAF25A4A}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="114" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1005,25 +1047,25 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="16">
         <v>1</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1043,7 +1085,7 @@
       <c r="E7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>34</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1074,7 +1116,7 @@
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="2">
@@ -1094,7 +1136,7 @@
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>47</v>
       </c>
       <c r="C10" s="2">
@@ -1143,13 +1185,13 @@
       <c r="C12" s="1">
         <v>5</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <v>200</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="8" t="s">
         <v>60</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1163,13 +1205,13 @@
       <c r="C13" s="2">
         <v>2</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>63</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="8" t="s">
         <v>65</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1183,13 +1225,13 @@
       <c r="C14" s="1">
         <v>16</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>68</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="8" t="s">
         <v>70</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -1197,48 +1239,48 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="23" t="s">
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="24" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8" t="s">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="10"/>
       <c r="C17" s="2"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C18" s="2"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>74</v>
       </c>
@@ -1252,71 +1294,71 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="11" t="s">
+      <c r="E20" s="7"/>
+      <c r="F20" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="19" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="20">
         <v>1</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="12" t="s">
+      <c r="G21" s="10"/>
+      <c r="H21" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="10">
         <v>1</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="G22" s="25"/>
-      <c r="H22" s="9" t="s">
+      <c r="G22" s="26"/>
+      <c r="H22" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>77</v>
       </c>
@@ -1329,54 +1371,73 @@
       <c r="E23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G23" s="14"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="9"/>
+      <c r="B24" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
+    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="10">
         <v>1</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9" t="s">
+      <c r="E27" s="10"/>
+      <c r="F27" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H27" s="18" t="s">
+      <c r="H27" s="19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="24" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="5">
+      <c r="B41" s="6">
         <v>190160099</v>
       </c>
       <c r="C41" s="1">
@@ -1388,7 +1449,7 @@
       <c r="E41" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="8" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1408,6 +1469,7 @@
     <hyperlink ref="F5" r:id="rId12" xr:uid="{FA5DA2F8-8B34-A647-B413-30133DA5F6B0}"/>
     <hyperlink ref="F8" r:id="rId13" xr:uid="{630F37CB-1E8B-C946-90D0-AF7758D45495}"/>
     <hyperlink ref="F10" r:id="rId14" xr:uid="{B9F04E2E-FE2B-014F-A271-AD9B481F131C}"/>
+    <hyperlink ref="F27" r:id="rId15" xr:uid="{951D4A0F-6B66-B347-BB83-79D1699FA1F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>